<commit_message>
ADD : 160 TRIALS PER BLOCK, NEW CONDITIPONS FILE, CounterBalancing
- Now each block has 160 trials
- A new conditions file with all 160 images and Arousal Codes.
- Two files to counter balance.

Now the two files to run are GroupA.psyexp and GroupB.psyexp
</commit_message>
<xml_diff>
--- a/block1_distractors.xlsx
+++ b/block1_distractors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pushkarsingh/Documents/01 University/03 Self Prioritisation Research/experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD986F1-1FB1-E045-9DA3-BF68AF795FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE73E5B-B07B-CF42-B7AE-C003229587B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="2000" windowWidth="26840" windowHeight="14760" xr2:uid="{D3DB7413-E5FE-AF48-AAC8-4C8C9B29E042}"/>
   </bookViews>
@@ -650,7 +650,7 @@
   <dimension ref="A1:C81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>